<commit_message>
[TicketUtil] Update RenewTicket and OpenCloseTicket to match current format
</commit_message>
<xml_diff>
--- a/config/TicketLogFromEmail.xlsx
+++ b/config/TicketLogFromEmail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/518289307e96aafe/Documents/VBAScripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_FAF7225C464B7444CAD13673199C5730616DDEA6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC5BA850-E203-421D-9587-C9DB5BC95581}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="11_FAF7225C464B7444CAD13673199C5730616DDEA6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86EE7CC3-61D1-4AE9-BBCB-12B37E279D0A}"/>
   <bookViews>
-    <workbookView xWindow="4692" yWindow="0" windowWidth="15900" windowHeight="12240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,25 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Email!$A$1:$G$80</definedName>
-    <definedName name="Contains">Config!$B$4:$I$4</definedName>
-    <definedName name="FilterOut">Config!$B$5:$E$5</definedName>
-    <definedName name="Flag">Config!$B$9:$B$10</definedName>
-    <definedName name="FlagKeywords">Config!$C$9:$D$10</definedName>
-    <definedName name="Folder">Config!$B$3</definedName>
-    <definedName name="FromEmail">Config!$B$2:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Email!$A$1:$H$2</definedName>
+    <definedName name="Assignee">Email!$E:$E</definedName>
+    <definedName name="Contains">Config!$B$5:$I$5</definedName>
+    <definedName name="ExpectedDateTime">Email!$H:$H</definedName>
+    <definedName name="FilterOut">Config!$B$6:$E$6</definedName>
+    <definedName name="Flag">Config!$B$10:$B$11</definedName>
+    <definedName name="FlagKeywords">Config!$C$10:$D$11</definedName>
+    <definedName name="Folder">Config!$B$4</definedName>
+    <definedName name="FromEmail">Config!$B$3:$H$3</definedName>
     <definedName name="Important">Email!$C:$C</definedName>
-    <definedName name="LastRunDateTime">Config!$B$12</definedName>
+    <definedName name="LastRunDateTime">Config!$B$13</definedName>
     <definedName name="LoginEmail">Config!$B$1</definedName>
+    <definedName name="Name">Config!$B$2</definedName>
     <definedName name="ReceivedDateTime">Email!$B:$B</definedName>
-    <definedName name="SearchLimit">Config!$B$6</definedName>
+    <definedName name="SearchLimit">Config!$B$7</definedName>
+    <definedName name="Status">Email!$F:$F</definedName>
     <definedName name="Subject">Email!$D:$D</definedName>
     <definedName name="TicketNum">Email!$A:$A</definedName>
+    <definedName name="UpdateDateTime">Email!$G:$G</definedName>
     <definedName name="Z_5907F90A_BF5B_4A6B_B9CB_41A7A0E318EF_.wvu.FilterData" localSheetId="1" hidden="1">Email!$A$1:$G$80</definedName>
     <definedName name="Z_6FD835F1_871F_443D_AE3E_387375420CD5_.wvu.FilterData" localSheetId="1" hidden="1">Email!$A$1:$G$74</definedName>
     <definedName name="Z_7AD2F51B_F34A_475B_9541_11CE09990102_.wvu.FilterData" localSheetId="1" hidden="1">Email!$A$1:$G$42</definedName>
@@ -64,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Folder</t>
   </si>
@@ -133,19 +138,42 @@
   </si>
   <si>
     <t>&lt;Your email&gt;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>&lt;Names of email accounts to receive from&gt;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>important</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Important</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Your name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Your name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Your name&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Please help with IT issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Expected finish date time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -162,12 +190,6 @@
       <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -186,6 +208,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -210,20 +238,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -264,13 +293,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>91440</xdr:colOff>
-          <xdr:row>13</xdr:row>
+          <xdr:row>14</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>1729740</xdr:colOff>
-          <xdr:row>15</xdr:row>
+          <xdr:row>16</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -303,7 +332,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="36576" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -314,8 +343,8 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Calibri"/>
-                  <a:cs typeface="Calibri"/>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
                 </a:rPr>
                 <a:t>Log tickets</a:t>
               </a:r>
@@ -610,10 +639,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -639,77 +668,85 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B13" s="3">
         <v>44742.409803240742</v>
       </c>
     </row>
@@ -731,7 +768,7 @@
       <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId4"/>
   <drawing r:id="rId5"/>
@@ -747,13 +784,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>91440</xdr:colOff>
-                    <xdr:row>13</xdr:row>
+                    <xdr:row>14</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>1729740</xdr:colOff>
-                    <xdr:row>15</xdr:row>
+                    <xdr:row>16</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </to>
                 </anchor>
@@ -770,11 +807,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -782,14 +819,15 @@
     <col min="1" max="1" width="3" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.375" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.625" style="8" customWidth="1"/>
     <col min="7" max="7" width="21.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.75" style="6"/>
+    <col min="8" max="8" width="34.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.75" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -811,74 +849,94 @@
       <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
+      <c r="H1" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>44745</v>
+      </c>
       <c r="C2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="9">
+        <v>44745</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
     </row>
@@ -1145,6 +1203,7 @@
       <c r="C80" s="7"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H2" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <customSheetViews>
     <customSheetView guid="{C11EE573-E01A-441B-9FF0-C456DDA64BDB}" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
@@ -1165,7 +1224,7 @@
       <autoFilter ref="A1:G80" xr:uid="{B888B65C-5739-40E6-8DFE-EEE06D023A58}"/>
     </customSheetView>
   </customSheetViews>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Y"</formula>

</xml_diff>

<commit_message>
[TicketUtil] Add image to explain named column
</commit_message>
<xml_diff>
--- a/config/TicketLogFromEmail.xlsx
+++ b/config/TicketLogFromEmail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/518289307e96aafe/Documents/VBAScripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="11_FAF7225C464B7444CAD13673199C5730616DDEA6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86EE7CC3-61D1-4AE9-BBCB-12B37E279D0A}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="11_FAF7225C464B7444CAD13673199C5730616DDEA6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E888F88-A815-497C-A816-0434EF9F4121}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7236" yWindow="0" windowWidth="15900" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,9 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
+    <customWorkbookView name="Yeung, Adriel - Personal View" guid="{5907F90A-BF5B-4A6B-B9CB-41A7A0E318EF}" mergeInterval="0" personalView="1" xWindow="-860" yWindow="-1477" windowWidth="1716" windowHeight="1271" activeSheetId="1"/>
+    <customWorkbookView name="Terry Lau    HKGH4 - Personal View" guid="{B9051402-BDBD-4BAB-B36A-8051CD7FA006}" mergeInterval="0" personalView="1" xWindow="-63" yWindow="-1103" windowWidth="1694" windowHeight="962" activeSheetId="2"/>
     <customWorkbookView name="Leung, Ringo      HKG16 - Personal View" guid="{C11EE573-E01A-441B-9FF0-C456DDA64BDB}" mergeInterval="0" personalView="1" maximized="1" xWindow="2869" yWindow="-11" windowWidth="3862" windowHeight="1582" activeSheetId="2"/>
-    <customWorkbookView name="Terry Lau    HKGH4 - Personal View" guid="{B9051402-BDBD-4BAB-B36A-8051CD7FA006}" mergeInterval="0" personalView="1" xWindow="-63" yWindow="-1103" windowWidth="1694" windowHeight="962" activeSheetId="2"/>
-    <customWorkbookView name="Yeung, Adriel - Personal View" guid="{5907F90A-BF5B-4A6B-B9CB-41A7A0E318EF}" mergeInterval="0" personalView="1" xWindow="-860" yWindow="-1477" windowWidth="1716" windowHeight="1271" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -89,9 +89,6 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>Limit to first # chars</t>
-  </si>
-  <si>
     <t>follow up</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
   </si>
   <si>
     <t>was assigned</t>
-  </si>
-  <si>
-    <t>Subject filter out</t>
   </si>
   <si>
     <t>RE:</t>
@@ -173,6 +167,14 @@
   </si>
   <si>
     <t>Expected finish date time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subject filter out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Limit to first # chars</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -641,8 +643,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -663,15 +665,15 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -679,7 +681,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -695,32 +697,32 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2">
         <v>400</v>
@@ -728,23 +730,23 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="3">
         <v>44742.409803240742</v>
@@ -752,8 +754,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C11EE573-E01A-441B-9FF0-C456DDA64BDB}" state="hidden">
-      <selection activeCell="B7" sqref="B7"/>
+    <customSheetView guid="{5907F90A-BF5B-4A6B-B9CB-41A7A0E318EF}">
+      <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
     </customSheetView>
@@ -762,8 +764,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{5907F90A-BF5B-4A6B-B9CB-41A7A0E318EF}">
-      <selection activeCell="B9" sqref="B9"/>
+    <customSheetView guid="{C11EE573-E01A-441B-9FF0-C456DDA64BDB}" state="hidden">
+      <selection activeCell="B7" sqref="B7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
     </customSheetView>
@@ -809,16 +811,16 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.875" style="8" customWidth="1"/>
     <col min="5" max="5" width="15.875" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.625" style="8" customWidth="1"/>
@@ -829,28 +831,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -862,16 +864,19 @@
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G2" s="9">
         <v>44745</v>
+      </c>
+      <c r="H2" s="9">
+        <v>44749</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1205,23 +1210,23 @@
   </sheetData>
   <autoFilter ref="A1:H2" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <customSheetViews>
-    <customSheetView guid="{C11EE573-E01A-441B-9FF0-C456DDA64BDB}" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G63" sqref="G63"/>
+    <customSheetView guid="{5907F90A-BF5B-4A6B-B9CB-41A7A0E318EF}" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:F74" xr:uid="{33671D60-C33D-406E-A2B6-091C40CC5E79}"/>
+      <autoFilter ref="A1:G80" xr:uid="{B843188B-0DD4-49E9-AD84-10175BCABB19}"/>
     </customSheetView>
     <customSheetView guid="{B9051402-BDBD-4BAB-B36A-8051CD7FA006}" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:F42" xr:uid="{295336EE-9F91-4F22-8C5B-F5CA7C149244}"/>
+      <autoFilter ref="A1:F42" xr:uid="{43A96365-A7E4-4D21-A646-346BA8CA8577}"/>
     </customSheetView>
-    <customSheetView guid="{5907F90A-BF5B-4A6B-B9CB-41A7A0E318EF}" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
+    <customSheetView guid="{C11EE573-E01A-441B-9FF0-C456DDA64BDB}" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G63" sqref="G63"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:G80" xr:uid="{B888B65C-5739-40E6-8DFE-EEE06D023A58}"/>
+      <autoFilter ref="A1:F74" xr:uid="{3F6FA469-B5A1-4F0C-B524-B7F02C5B1A7D}"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>